<commit_message>
Major Fix including Ftp Upload
</commit_message>
<xml_diff>
--- a/src/App/Reports/Payroll_Summary.xlsx
+++ b/src/App/Reports/Payroll_Summary.xlsx
@@ -921,7 +921,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1040,8 +1040,7 @@
 Page &amp;P/&amp;N&amp;C&amp;"Calibri,Bold"&amp;12MEGABYTE COLLEGE, INC.
 &amp;"Calibri,Regular"&amp;10Floridablanca, Pampanga
 &amp;14PAYROLL SUMMARY&amp;"Calibri,Bold"&amp;12
-&amp;"Calibri,Italic"&amp;11%Title%&amp;9
-%Title2%</oddHeader>
+&amp;"Calibri,Italic"&amp;11%Title%</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>